<commit_message>
feat: Add `pengujian` database schema and Excel data processing module with BEBAN calculation logic.
</commit_message>
<xml_diff>
--- a/Data Input Pengujian/data.xlsx
+++ b/Data Input Pengujian/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\odooCompressionTest\Data Input Pengujian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCC323D-52B0-4455-9D05-4C5CA42A721F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34B7D20-BF56-43A7-A1BB-30F404D6CD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="79">
   <si>
     <t>Tanggal</t>
   </si>
@@ -76,9 +76,6 @@
     <t>TM 906</t>
   </si>
   <si>
-    <t>TM 944</t>
-  </si>
-  <si>
     <t>TAUFIQ</t>
   </si>
   <si>
@@ -94,124 +91,175 @@
     <t>TM 813</t>
   </si>
   <si>
-    <t>Class E-1 NFA</t>
-  </si>
-  <si>
     <t>NANDA</t>
   </si>
   <si>
-    <t>2025-12-02</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/26718</t>
-  </si>
-  <si>
-    <t>HK - JAKON JO / HALFSLAB PS 14 STA 30+800 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
     <t>TM 648</t>
   </si>
   <si>
-    <t>2025-12-02 15:10:36</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/26730</t>
-  </si>
-  <si>
-    <t>2025-12-02 17:56:12</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/26697</t>
-  </si>
-  <si>
-    <t>PT SRA / K 350 / AD PTB</t>
-  </si>
-  <si>
-    <t>Proyek Pekerjaan Fasilitas Workshop PGT Patimban</t>
-  </si>
-  <si>
-    <t>K-350 NFA</t>
-  </si>
-  <si>
-    <t>2025-12-02 08:44:56</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/26701</t>
-  </si>
-  <si>
-    <t>WIKA-ADHI JO / LC AKSES DETOUR / CLASS E / AD PTB</t>
-  </si>
-  <si>
-    <t>2025-12-02 10:13:22</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/26708</t>
-  </si>
-  <si>
-    <t>2025-12-02 11:42:00</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/26729</t>
-  </si>
-  <si>
-    <t>WIKA-ADHI JO / PARAPET SPAN 8 - 9W IC 02 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>2025-12-02 17:47:37</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/26735</t>
-  </si>
-  <si>
     <t>TM 782</t>
   </si>
   <si>
-    <t>2025-12-02 19:30:28</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/26699</t>
-  </si>
-  <si>
-    <t>WIKA-ADHI JO / PLATFORM SLAB P15 - A2 MB 22 / CLASS E / AD PTBI JO</t>
-  </si>
-  <si>
     <t>EGI</t>
   </si>
   <si>
-    <t>2025-12-02 09:43:00</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/26705</t>
-  </si>
-  <si>
-    <t>2025-12-02 10:55:30</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/26722</t>
-  </si>
-  <si>
-    <t>WIKA-ADHI JO / SLAB EEJ3 - E4E PS 17 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>2025-12-02 17:01:51</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/26724</t>
-  </si>
-  <si>
     <t>TM 690</t>
   </si>
   <si>
-    <t>2025-12-02 17:05:21</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/26731</t>
-  </si>
-  <si>
     <t>DENI</t>
   </si>
   <si>
-    <t>2025-12-02 18:04:09</t>
+    <t>2025-12-03</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26768</t>
+  </si>
+  <si>
+    <t>HK - JAKON JO / DIAFRAGMA AW1 - PW1 BRIDGE 17 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>2025-12-03 11:28:09</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26772</t>
+  </si>
+  <si>
+    <t>2025-12-03 12:18:04</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26775</t>
+  </si>
+  <si>
+    <t>NK / LANTAI / K 300 / AD PTB</t>
+  </si>
+  <si>
+    <t>Pekerjaan Siphon Sisi Timur Bendung Salamdarma</t>
+  </si>
+  <si>
+    <t>K-300 NFA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Slump 10.0 +2.0/-2.0</t>
+  </si>
+  <si>
+    <t>TM 965</t>
+  </si>
+  <si>
+    <t>2025-12-03 13:53:51</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26787</t>
+  </si>
+  <si>
+    <t>2025-12-03 15:45:44</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26761</t>
+  </si>
+  <si>
+    <t>WIKA-ADHI JO / DECKSLAB RAMP 7 IC 05 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>2025-12-03 10:13:46</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26765</t>
+  </si>
+  <si>
+    <t>2025-12-03 10:54:01</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26803</t>
+  </si>
+  <si>
+    <t>WIKA-ADHI JO / PIERHEAD P5W MB 25 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>2025-12-03 19:13:32</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26806</t>
+  </si>
+  <si>
+    <t>2025-12-03 19:44:28</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26818</t>
+  </si>
+  <si>
+    <t>WIKA-ADHI JO / SLAB E4E - EEJ4 PS 17 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>2025-12-03 21:53:34</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26821</t>
+  </si>
+  <si>
+    <t>2025-12-03 22:06:28</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26825</t>
+  </si>
+  <si>
+    <t>TM 496</t>
+  </si>
+  <si>
+    <t>2025-12-03 23:52:45</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26814</t>
+  </si>
+  <si>
+    <t>WIKA-ADHI JO / SLAB P13 - P14W MB 22 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>2025-12-03 21:26:10</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26822</t>
+  </si>
+  <si>
+    <t>2025-12-03 23:21:55</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26824</t>
+  </si>
+  <si>
+    <t>2025-12-03 23:46:21</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26776</t>
+  </si>
+  <si>
+    <t>WIKA-ADHI JO / SLAB P8 - P7E MB 22 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>2025-12-03 14:05:28</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26780</t>
+  </si>
+  <si>
+    <t>2025-12-03 14:40:16</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26790</t>
+  </si>
+  <si>
+    <t>TM 902</t>
+  </si>
+  <si>
+    <t>2025-12-03 16:31:06</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26789</t>
+  </si>
+  <si>
+    <t>WIKA-ADHI JO / SLEEPER BOX RAMP 4 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>2025-12-03 16:25:21</t>
   </si>
 </sst>
 </file>
@@ -588,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,51 +681,51 @@
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>8</v>
@@ -686,111 +734,111 @@
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="I6" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>9</v>
@@ -799,27 +847,27 @@
         <v>8</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>9</v>
@@ -828,18 +876,18 @@
         <v>8</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>49</v>
@@ -848,10 +896,10 @@
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>8</v>
@@ -860,53 +908,53 @@
         <v>14</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>9</v>
@@ -915,27 +963,27 @@
         <v>8</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>9</v>
@@ -944,27 +992,27 @@
         <v>8</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>9</v>
@@ -976,7 +1024,181 @@
         <v>15</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>62</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add Excel data processing module with functionality to load data, check row duplication, and calculate BEBAN values based on specific criteria.
</commit_message>
<xml_diff>
--- a/Data Input Pengujian/data.xlsx
+++ b/Data Input Pengujian/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\odooCompressionTest\Data Input Pengujian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34B7D20-BF56-43A7-A1BB-30F404D6CD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DCFFA3-9F84-4010-8C30-460907D040D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="107">
   <si>
     <t>Tanggal</t>
   </si>
@@ -260,6 +260,90 @@
   </si>
   <si>
     <t>2025-12-03 16:25:21</t>
+  </si>
+  <si>
+    <t>2025-12-04</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26867</t>
+  </si>
+  <si>
+    <t>HK - JAKON JO / DECKSLAB A1 - P OP 5 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>2025-12-04 08:55:21</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26869</t>
+  </si>
+  <si>
+    <t>TM 601</t>
+  </si>
+  <si>
+    <t>2025-12-04 09:36:50</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26883</t>
+  </si>
+  <si>
+    <t>2025-12-04 19:57:37</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26864</t>
+  </si>
+  <si>
+    <t>HK - JAKON JO / LC A2 OP 7 / CLASS E / AD PTB</t>
+  </si>
+  <si>
+    <t>Class E-1 FA</t>
+  </si>
+  <si>
+    <t>2025-12-04 08:25:26</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26865</t>
+  </si>
+  <si>
+    <t>TM 944</t>
+  </si>
+  <si>
+    <t>2025-12-04 08:31:24</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26880</t>
+  </si>
+  <si>
+    <t>PT SRA / K 350 / AD PTB</t>
+  </si>
+  <si>
+    <t>Proyek Pekerjaan Fasilitas Workshop PGT Patimban</t>
+  </si>
+  <si>
+    <t>SUGENG</t>
+  </si>
+  <si>
+    <t>K-350 NFA</t>
+  </si>
+  <si>
+    <t>2025-12-04 14:01:51</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26875</t>
+  </si>
+  <si>
+    <t>WASKITA - ABP JO / BARRIER GRID AE2 - PE1' STA 25+949 - 25+896 SISI MEDIAN &amp; LUAR / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>Patimban Access Toll Road P02 (JOI 60%)</t>
+  </si>
+  <si>
+    <t>2025-12-04 11:41:00</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/26881</t>
+  </si>
+  <si>
+    <t>2025-12-04 14:11:17</t>
   </si>
 </sst>
 </file>
@@ -636,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,6 +1285,238 @@
         <v>78</v>
       </c>
     </row>
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: Add various Excel reports, data files, planning documents, and image assets.
</commit_message>
<xml_diff>
--- a/Data Input Pengujian/data.xlsx
+++ b/Data Input Pengujian/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\odooCompressionTest\Data Input Pengujian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C9F186-04ED-45BF-A8F0-4CB5FE0EA2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA9F937-7433-4B0D-AA72-B7B137E20F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="100">
   <si>
     <t>Tanggal</t>
   </si>
@@ -61,217 +61,268 @@
     <t>Class B-1 NFA</t>
   </si>
   <si>
+    <t>DENI</t>
+  </si>
+  <si>
+    <t>TM 813</t>
+  </si>
+  <si>
+    <t>TM 648</t>
+  </si>
+  <si>
+    <t>Pembangunan Jalan Tol  Akses Patimban Paket 3</t>
+  </si>
+  <si>
+    <t>Class B-1 FA</t>
+  </si>
+  <si>
+    <t>TM 967</t>
+  </si>
+  <si>
+    <t>TM 690</t>
+  </si>
+  <si>
+    <t>TM 944</t>
+  </si>
+  <si>
+    <t>TM 496</t>
+  </si>
+  <si>
+    <t>AGUS</t>
+  </si>
+  <si>
+    <t>TM 531</t>
+  </si>
+  <si>
+    <t>Class B-2 NFA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Slump 55.0 +10.0/-0.0</t>
+  </si>
+  <si>
+    <t>NANDA</t>
+  </si>
+  <si>
+    <t>2025-12-27</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28328</t>
+  </si>
+  <si>
+    <t>WIKA - ADHI JO / BP P2E 2E MB 21 / CLASS B-2 SCC / AD PTB</t>
+  </si>
+  <si>
+    <t>2025-12-27 18:31:37</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28332</t>
+  </si>
+  <si>
+    <t>TM 906</t>
+  </si>
+  <si>
+    <t>2025-12-27 19:19:22</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28324</t>
+  </si>
+  <si>
+    <t>WIKA - ADHI JO / PARAPET OUTER W4G - W5G PS 17 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>2025-12-27 16:48:44</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28326</t>
+  </si>
+  <si>
+    <t>2025-12-27 17:16:40</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28315</t>
+  </si>
+  <si>
+    <t>WIKA - ADHI JO / PARAPET SPAN 1, 2E OUTER IC 02 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>ARDIAN</t>
+  </si>
+  <si>
+    <t>2025-12-27 09:13:33</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28317</t>
+  </si>
+  <si>
+    <t>2025-12-27 10:27:25</t>
+  </si>
+  <si>
+    <t>2025-12-28</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28368</t>
+  </si>
+  <si>
+    <t>HK - JAKON JO / BARRIER TOP SLAB A97 - AE1 (R/L) PS 14 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>2025-12-28 20:19:16</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28371</t>
+  </si>
+  <si>
+    <t>TM 965</t>
+  </si>
+  <si>
+    <t>2025-12-28 21:14:05</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28375</t>
+  </si>
+  <si>
+    <t>2025-12-28 22:15:08</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28359</t>
+  </si>
+  <si>
+    <t>WIKA - ADHI JO / BP P2E 2S MB 21 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
     <t>TAUFIQ</t>
   </si>
   <si>
-    <t>Pembangunan Jalan Tol  Akses Patimban Paket 3</t>
-  </si>
-  <si>
-    <t>TM 690</t>
-  </si>
-  <si>
-    <t>TM 965</t>
-  </si>
-  <si>
-    <t>DENI</t>
-  </si>
-  <si>
-    <t>TM 601</t>
-  </si>
-  <si>
-    <t>AGUS</t>
-  </si>
-  <si>
-    <t>TM 906</t>
+    <t>2025-12-28 18:05:48</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28363</t>
+  </si>
+  <si>
+    <t>2025-12-28 18:53:33</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28337</t>
+  </si>
+  <si>
+    <t>WIKA - ADHI JO / RC SLAB P2 - P1W MB 22 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>2025-12-28 12:57:38</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28343</t>
+  </si>
+  <si>
+    <t>2025-12-28 14:05:59</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28349</t>
+  </si>
+  <si>
+    <t>2025-12-28 15:43:16</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28354</t>
+  </si>
+  <si>
+    <t>2025-12-28 16:45:12</t>
+  </si>
+  <si>
+    <t>2025-12-29</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28397</t>
+  </si>
+  <si>
+    <t>HK - JAKON JO / LC PH PS 11 STA 28+000 / CLASS E / AD PTB</t>
+  </si>
+  <si>
+    <t>SUGENG</t>
+  </si>
+  <si>
+    <t>Class E-1 FA</t>
+  </si>
+  <si>
+    <t>2025-12-29 14:14:43</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28377</t>
+  </si>
+  <si>
+    <t>WIKA - ADHI JO / RC SLAB P2 - P1E MB 22 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>2025-12-29 09:29:54</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28383</t>
+  </si>
+  <si>
+    <t>2025-12-29 10:39:49</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28390</t>
+  </si>
+  <si>
+    <t>2025-12-29 12:11:53</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28395</t>
+  </si>
+  <si>
+    <t>2025-12-29 13:15:10</t>
+  </si>
+  <si>
+    <t>2025-12-30</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28416</t>
+  </si>
+  <si>
+    <t>HK - JAKON JO / HALFSLAB TYPE S3.1 (8 UNIT), S1AD (8 UNIT) + SLEEPER / CLASS B-1 / AD PTB</t>
   </si>
   <si>
     <t>TM 782</t>
   </si>
   <si>
-    <t>DATA</t>
-  </si>
-  <si>
-    <t>TM 813</t>
-  </si>
-  <si>
-    <t>TM 944</t>
-  </si>
-  <si>
-    <t>EGI</t>
-  </si>
-  <si>
-    <t>WASKITA - ABP JO / TIANG &amp; PAGAR PANEL / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>Patimban Access Toll Road P02 (JOI 60%)</t>
-  </si>
-  <si>
-    <t>TM 631</t>
-  </si>
-  <si>
-    <t>NANDA</t>
-  </si>
-  <si>
-    <t>WIKA - ADHI JO / PILESLAB E7E - EEJ7 PS 17 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>2025-12-23</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28073</t>
-  </si>
-  <si>
-    <t>HK - JAKON JO / TOP SLAB L1 - L10 OP 5 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>Class B-1 FA</t>
-  </si>
-  <si>
-    <t>2025-12-23 10:53:44</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28076</t>
-  </si>
-  <si>
-    <t>2025-12-23 11:15:23</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28100</t>
-  </si>
-  <si>
-    <t>TM 531</t>
-  </si>
-  <si>
-    <t>2025-12-23 18:27:10</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28129</t>
-  </si>
-  <si>
-    <t>2025-12-23 23:58:19</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28089</t>
-  </si>
-  <si>
-    <t>PP - TOL PTB / DINDING WW INLET BC STA 17+875 / FC 30 / AD PTB</t>
-  </si>
-  <si>
-    <t>JALAN TOL AKSES PATIMBAN</t>
-  </si>
-  <si>
-    <t>Fc-30 NFA</t>
-  </si>
-  <si>
-    <t>2025-12-23 15:35:07</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28069</t>
-  </si>
-  <si>
-    <t>PP - TOL PTB / LC APPROACH BC STA 17+060 / K 125 / AD PTB</t>
-  </si>
-  <si>
-    <t>K-125 NFA</t>
-  </si>
-  <si>
-    <t>2025-12-23 09:59:23</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28070</t>
-  </si>
-  <si>
-    <t>PP - TOL PTB / LC PILECAPE B3 STA 18+319 / K 125 / AD PTB</t>
-  </si>
-  <si>
-    <t>TM 496</t>
-  </si>
-  <si>
-    <t>2025-12-23 10:18:00</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28071</t>
-  </si>
-  <si>
-    <t>2025-12-23 10:23:10</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28068</t>
-  </si>
-  <si>
-    <t>SUGENG</t>
-  </si>
-  <si>
-    <t>2025-12-23 09:48:23</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28082</t>
-  </si>
-  <si>
-    <t>WIKA - ADHI JO / PIERHEAD P3W STG 2 MB 25 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>2025-12-23 13:52:57</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28085</t>
-  </si>
-  <si>
-    <t>2025-12-23 14:56:26</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28064</t>
-  </si>
-  <si>
-    <t>2025-12-23 01:25:17</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28067</t>
-  </si>
-  <si>
-    <t>2025-12-23 03:10:00</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28123</t>
-  </si>
-  <si>
-    <t>WIKA - ADHI JO / PILESLAB EEJ6 - E7E PS 17 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>2025-12-23 22:59:08</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28124</t>
-  </si>
-  <si>
-    <t>2025-12-23 23:06:50</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28103</t>
-  </si>
-  <si>
-    <t>WIKA - ADHI JO / RC SLAB P4 - P3E MB 22 / CLASS B-1 / AD PTB</t>
-  </si>
-  <si>
-    <t>2025-12-23 19:06:18</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28107</t>
-  </si>
-  <si>
-    <t>2025-12-23 20:24:33</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28116</t>
-  </si>
-  <si>
-    <t>2025-12-23 21:41:37</t>
-  </si>
-  <si>
-    <t>DOCKET/PTB/12-2025/28121</t>
-  </si>
-  <si>
-    <t>2025-12-23 22:35:02</t>
+    <t>2025-12-30 15:36:38</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28418</t>
+  </si>
+  <si>
+    <t>TM 494</t>
+  </si>
+  <si>
+    <t>2025-12-30 15:59:41</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28399</t>
+  </si>
+  <si>
+    <t>HK - JAKON JO / PILECAPE A1 OP 7 / CLASS B-1 / AD PTB</t>
+  </si>
+  <si>
+    <t>2025-12-30 10:48:43</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28403</t>
+  </si>
+  <si>
+    <t>2025-12-30 11:28:13</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28410</t>
+  </si>
+  <si>
+    <t>2025-12-30 13:04:11</t>
+  </si>
+  <si>
+    <t>DOCKET/PTB/12-2025/28414</t>
+  </si>
+  <si>
+    <t>2025-12-30 14:18:46</t>
   </si>
 </sst>
 </file>
@@ -648,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,140 +742,140 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>8</v>
@@ -833,198 +884,198 @@
         <v>14</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="2" t="s">
+    </row>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>11</v>
@@ -1033,27 +1084,27 @@
         <v>8</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>11</v>
@@ -1062,27 +1113,27 @@
         <v>8</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>11</v>
@@ -1091,27 +1142,27 @@
         <v>8</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>11</v>
@@ -1120,47 +1171,47 @@
         <v>8</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="E17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>75</v>
@@ -1169,7 +1220,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>11</v>
@@ -1178,18 +1229,18 @@
         <v>8</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>75</v>
@@ -1198,7 +1249,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>11</v>
@@ -1207,18 +1258,18 @@
         <v>8</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>75</v>
@@ -1227,7 +1278,7 @@
         <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>11</v>
@@ -1239,7 +1290,210 @@
         <v>20</v>
       </c>
       <c r="I20" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>